<commit_message>
sep public with private
</commit_message>
<xml_diff>
--- a/DataWrangling/Classification_ZZ.xlsx
+++ b/DataWrangling/Classification_ZZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhizh\OneDrive - Stop TB Partnership\UNOPS\10 Paper Writing\CAR software\02 Bangladesh\MachineBGD\DataWrangling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stoptb-my.sharepoint.com/personal/zhizhenq_stoptb_org/Documents/UNOPS/10 Paper Writing/CAR software/02 Bangladesh/MachineBGD/DataWrangling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{FD20D8CE-D3C8-4050-B4F0-018015F9B62C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FCF93AF-8F11-47E8-9F16-20F62AA6A282}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{FD20D8CE-D3C8-4050-B4F0-018015F9B62C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C8AD19BC-7427-4E4D-B776-D284DA1B9907}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>Screening</t>
   </si>
@@ -240,10 +240,13 @@
     <t>WalkIn</t>
   </si>
   <si>
-    <t>PrivatePublicReferral</t>
-  </si>
-  <si>
     <t>PublicDOTSRetesting</t>
+  </si>
+  <si>
+    <t>PublicReferral</t>
+  </si>
+  <si>
+    <t>PrivateReferral</t>
   </si>
 </sst>
 </file>
@@ -661,10 +664,10 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B47"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,123 +741,123 @@
       <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
+      <c r="A12" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
+      <c r="A14" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C14" s="9"/>
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>61</v>
@@ -862,321 +865,321 @@
       <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>17</v>
+      <c r="A17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>19</v>
+      <c r="A18" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="14"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="13" t="s">
+      <c r="A44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="4"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="15" t="s">
+      <c r="B47" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="14"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="4"/>
       <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1267,12 +1270,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062475C3A4A48CB43BEEF02300CCB0B94" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b03845c670f425a50532542b24f28658">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0165605e-33a8-4c1d-8b96-6494f482604e" xmlns:ns4="8b73d56b-a1f8-4aec-9bfa-4919f739c9f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d30c1d76703923a8dc578e7d1705bf5e" ns3:_="" ns4:_="">
     <xsd:import namespace="0165605e-33a8-4c1d-8b96-6494f482604e"/>
@@ -1495,6 +1492,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1505,15 +1508,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F334CA8-1832-4B10-A192-89F0F8C7D8D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F77C225-AD4F-4A69-9137-8D9712B91BE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1532,6 +1526,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F334CA8-1832-4B10-A192-89F0F8C7D8D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15E0D8B3-A55E-471C-BA09-0B058301A9FB}">
   <ds:schemaRefs>

</xml_diff>